<commit_message>
Funktionen für die Personen Auswahl udnnfür dwchsel dzwischen dr Login & Registrierungs Anzeigen erstellt + JavaFX Chat Übersicht gefertigt
</commit_message>
<xml_diff>
--- a/Projektdetails_WS24_Gruppe_7.xlsx
+++ b/Projektdetails_WS24_Gruppe_7.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skclk\Desktop\Informations- und Kommunikationssysteme\3.Semester\ODE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skclk\Desktop\Informations- und Kommunikationssysteme\3.Semester\ODE\ChatConnect_ODE-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{867DC11E-BA07-4371-9432-285C6505C705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48322696-DD25-4078-AF4A-B721924B00A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="158">
   <si>
     <t>Informationen</t>
   </si>
@@ -851,6 +851,33 @@
   <si>
     <t>Die Anmelde und Registrierungs anzeigen wurden im selben fxml Datei &amp; Controller implementiert. Für die Anzeige der Chatt Übersicht wurde eine extra fxml Datei &amp; Controller erstellt.</t>
   </si>
+  <si>
+    <t>Personen Auswahl</t>
+  </si>
+  <si>
+    <t>Chat Anzeige</t>
+  </si>
+  <si>
+    <t>Funktionen für die Anpassung der Anzeige an die Personen</t>
+  </si>
+  <si>
+    <t>Müsste mit weiteren Features erweitert werden</t>
+  </si>
+  <si>
+    <t>Eventuell durch weitere Features anpassungs bedarf</t>
+  </si>
+  <si>
+    <t>Swap von Login &amp; Registrations Anzeige</t>
+  </si>
+  <si>
+    <t>Funktionen mit der man zwischen der Login und Registrations Anzeige wechseln kann</t>
+  </si>
+  <si>
+    <t>Datenbank müsste noch damit verbunden werden</t>
+  </si>
+  <si>
+    <t>Design für die Chat Anzeige wurde verfeinert und gefertigt</t>
+  </si>
 </sst>
 </file>
 
@@ -1011,7 +1038,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1052,13 +1079,6 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1085,6 +1105,19 @@
     </xf>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4723,7 +4756,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="13.2">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="29" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="15" t="s">
@@ -4731,13 +4764,13 @@
       </c>
     </row>
     <row r="5" spans="2:3" ht="13.2">
-      <c r="B5" s="19"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="15" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="13.2">
-      <c r="B6" s="19"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="15" t="s">
         <v>131</v>
       </c>
@@ -4763,99 +4796,99 @@
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="2:3" ht="13.2">
-      <c r="B10" s="18" t="s">
+      <c r="B10" s="29" t="s">
         <v>64</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="18" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="30">
-      <c r="B11" s="19"/>
-      <c r="C11" s="22" t="s">
+      <c r="B11" s="30"/>
+      <c r="C11" s="19" t="s">
         <v>120</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="15">
-      <c r="B12" s="19"/>
-      <c r="C12" s="22" t="s">
+      <c r="B12" s="30"/>
+      <c r="C12" s="19" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="13.2">
-      <c r="B13" s="19"/>
-      <c r="C13" s="23"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="20"/>
     </row>
     <row r="14" spans="2:3" ht="15">
-      <c r="B14" s="18" t="s">
+      <c r="B14" s="29" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="22" t="s">
+      <c r="C14" s="19" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="15">
-      <c r="B15" s="19"/>
-      <c r="C15" s="22" t="s">
+      <c r="B15" s="30"/>
+      <c r="C15" s="19" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="15">
-      <c r="B16" s="19"/>
-      <c r="C16" s="22" t="s">
+      <c r="B16" s="30"/>
+      <c r="C16" s="19" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="13.2">
-      <c r="B17" s="19"/>
-      <c r="C17" s="23"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="20"/>
     </row>
     <row r="18" spans="2:3" ht="15">
-      <c r="B18" s="18" t="s">
+      <c r="B18" s="29" t="s">
         <v>66</v>
       </c>
-      <c r="C18" s="22" t="s">
+      <c r="C18" s="19" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="15">
-      <c r="B19" s="19"/>
-      <c r="C19" s="22" t="s">
+      <c r="B19" s="30"/>
+      <c r="C19" s="19" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="15">
-      <c r="B20" s="19"/>
-      <c r="C20" s="22" t="s">
+      <c r="B20" s="30"/>
+      <c r="C20" s="19" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="13.2">
-      <c r="B21" s="19"/>
-      <c r="C21" s="23"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="20"/>
     </row>
     <row r="22" spans="2:3" ht="15">
-      <c r="B22" s="18" t="s">
+      <c r="B22" s="29" t="s">
         <v>67</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="19" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="30">
-      <c r="B23" s="19"/>
-      <c r="C23" s="22" t="s">
+      <c r="B23" s="30"/>
+      <c r="C23" s="19" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="15">
-      <c r="B24" s="19"/>
-      <c r="C24" s="22" t="s">
+      <c r="B24" s="30"/>
+      <c r="C24" s="19" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="13.2">
-      <c r="B25" s="19"/>
+      <c r="B25" s="30"/>
       <c r="C25" s="10"/>
     </row>
     <row r="26" spans="2:3" ht="13.2">
@@ -8785,7 +8818,7 @@
   </sheetPr>
   <dimension ref="B1:G6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -8799,86 +8832,86 @@
     <col min="7" max="7" width="30.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="24" customFormat="1" ht="12.6" customHeight="1"/>
-    <row r="2" spans="2:7" s="27" customFormat="1" ht="13.2">
-      <c r="B2" s="26" t="s">
+    <row r="1" spans="2:7" s="21" customFormat="1" ht="12.6" customHeight="1"/>
+    <row r="2" spans="2:7" s="24" customFormat="1" ht="13.2">
+      <c r="B2" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="23" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="26" t="s">
+      <c r="D2" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="26" t="s">
+      <c r="E2" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="26" t="s">
+      <c r="F2" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="23" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" spans="2:7" s="27" customFormat="1" ht="15">
-      <c r="B3" s="27" t="s">
+    <row r="3" spans="2:7" s="24" customFormat="1" ht="15">
+      <c r="B3" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="22" t="s">
+      <c r="C3" s="19" t="s">
         <v>140</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="22" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="2:7" s="27" customFormat="1" ht="39.6">
-      <c r="B4" s="25" t="s">
+    <row r="4" spans="2:7" s="24" customFormat="1" ht="39.6">
+      <c r="B4" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="E4" s="27">
+      <c r="E4" s="24">
         <v>5</v>
       </c>
-      <c r="F4" s="25" t="s">
+      <c r="F4" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="G4" s="25" t="s">
+      <c r="G4" s="22" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="2:7" s="27" customFormat="1" ht="26.4">
-      <c r="B5" s="27" t="s">
+    <row r="5" spans="2:7" s="24" customFormat="1" ht="26.4">
+      <c r="B5" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>145</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="F5" s="25" t="s">
+      <c r="F5" s="22" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="6" spans="2:7" s="27" customFormat="1" ht="26.4">
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="2:7" s="24" customFormat="1" ht="26.4">
+      <c r="B6" s="22" t="s">
         <v>136</v>
       </c>
-      <c r="C6" s="29" t="s">
+      <c r="C6" s="26" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="F6" s="25" t="s">
+      <c r="F6" s="22" t="s">
         <v>147</v>
       </c>
     </row>
@@ -8892,39 +8925,110 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B2:G2"/>
+  <dimension ref="B2:G13"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5546875" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="3" max="3" width="15.44140625" customWidth="1"/>
-    <col min="4" max="4" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="34.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="71.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.5546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:7">
-      <c r="B2" s="12" t="s">
+    <row r="2" spans="2:7" s="28" customFormat="1" ht="13.2">
+      <c r="B2" s="27" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="D2" s="12" t="s">
+      <c r="D2" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="E2" s="12" t="s">
+      <c r="E2" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="F2" s="12" t="s">
+      <c r="F2" s="27" t="s">
         <v>72</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="27" t="s">
         <v>73</v>
       </c>
     </row>
+    <row r="3" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B3" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>151</v>
+      </c>
+      <c r="E3" s="28">
+        <v>2</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B4" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>150</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>157</v>
+      </c>
+      <c r="E4" s="28">
+        <v>1</v>
+      </c>
+      <c r="F4" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1">
+      <c r="B5" s="28" t="s">
+        <v>135</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>154</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>155</v>
+      </c>
+      <c r="E5" s="28">
+        <v>1</v>
+      </c>
+      <c r="F5" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="7" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="8" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="9" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="10" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="11" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="12" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="13" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9055,7 +9159,7 @@
       </c>
     </row>
     <row r="4" spans="2:3" ht="13.2">
-      <c r="B4" s="18" t="s">
+      <c r="B4" s="29" t="s">
         <v>60</v>
       </c>
       <c r="C4" s="10" t="s">
@@ -9063,13 +9167,13 @@
       </c>
     </row>
     <row r="5" spans="2:3" ht="13.2">
-      <c r="B5" s="19"/>
+      <c r="B5" s="30"/>
       <c r="C5" s="2" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="13.2">
-      <c r="B6" s="19"/>
+      <c r="B6" s="30"/>
       <c r="C6" s="2" t="s">
         <v>78</v>
       </c>
@@ -9095,7 +9199,7 @@
       <c r="C9" s="10"/>
     </row>
     <row r="10" spans="2:3" ht="13.2">
-      <c r="B10" s="20" t="s">
+      <c r="B10" s="31" t="s">
         <v>115</v>
       </c>
       <c r="C10" s="10" t="s">
@@ -9103,23 +9207,23 @@
       </c>
     </row>
     <row r="11" spans="2:3" ht="13.2">
-      <c r="B11" s="19"/>
+      <c r="B11" s="30"/>
       <c r="C11" s="10" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="13.2">
-      <c r="B12" s="19"/>
+      <c r="B12" s="30"/>
       <c r="C12" s="10" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="13.2">
-      <c r="B13" s="19"/>
+      <c r="B13" s="30"/>
       <c r="C13" s="10"/>
     </row>
     <row r="14" spans="2:3" ht="13.2">
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="31" t="s">
         <v>116</v>
       </c>
       <c r="C14" s="2" t="s">
@@ -9127,22 +9231,22 @@
       </c>
     </row>
     <row r="15" spans="2:3" ht="13.2">
-      <c r="B15" s="19"/>
+      <c r="B15" s="30"/>
       <c r="C15" s="2" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="13.2">
-      <c r="B16" s="19"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="2" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B17" s="19"/>
+      <c r="B17" s="30"/>
     </row>
     <row r="18" spans="2:3" ht="13.2">
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="31" t="s">
         <v>117</v>
       </c>
       <c r="C18" s="2" t="s">
@@ -9150,22 +9254,22 @@
       </c>
     </row>
     <row r="19" spans="2:3" ht="13.2">
-      <c r="B19" s="19"/>
+      <c r="B19" s="30"/>
       <c r="C19" s="2" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="13.2">
-      <c r="B20" s="19"/>
+      <c r="B20" s="30"/>
       <c r="C20" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B21" s="19"/>
+      <c r="B21" s="30"/>
     </row>
     <row r="22" spans="2:3" ht="13.2">
-      <c r="B22" s="20" t="s">
+      <c r="B22" s="31" t="s">
         <v>118</v>
       </c>
       <c r="C22" s="2" t="s">
@@ -9173,19 +9277,19 @@
       </c>
     </row>
     <row r="23" spans="2:3" ht="13.2">
-      <c r="B23" s="19"/>
+      <c r="B23" s="30"/>
       <c r="C23" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="13.2">
-      <c r="B24" s="19"/>
+      <c r="B24" s="30"/>
       <c r="C24" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15.75" customHeight="1">
-      <c r="B25" s="19"/>
+      <c r="B25" s="30"/>
     </row>
     <row r="26" spans="2:3" ht="13.2">
       <c r="B26" s="9"/>

</xml_diff>

<commit_message>
GUI Design verbessert und angepasst
</commit_message>
<xml_diff>
--- a/Projektdetails_WS24_Gruppe_7.xlsx
+++ b/Projektdetails_WS24_Gruppe_7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\skclk\Desktop\Informations- und Kommunikationssysteme\3.Semester\ODE\ChatConnect_ODE-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A320B72C-ADF3-4EA4-8421-A506CEE9F2CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{164C74FB-5395-4B94-A9B4-3BAA5807EC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="169">
   <si>
     <t>Informationen</t>
   </si>
@@ -414,76 +414,13 @@
     <t xml:space="preserve">    Keine anderen Libraries/Frameworks verwendet</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;Must have feature 1&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Must have feature 1&gt; getestet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Must have feature 2&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Must have feature 2&gt; getestet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Must have feature 3&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Must have feature 3&gt; getestet</t>
-  </si>
-  <si>
     <t>Should haves</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;Should have feature 1&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Should have feature 1&gt; getestet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Should have feature 2&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Should have feature 2&gt; getestet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Should have feature 3&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Should have feature 3&gt; getestet</t>
-  </si>
-  <si>
     <t>Nice to haves</t>
   </si>
   <si>
-    <t xml:space="preserve">    &lt;Nice to have feature 1&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Nice to have feature 1&gt; getestet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Nice to have feature 2&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Nice to have feature 2&gt; getestet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Nice to have feature 3&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Nice to have feature 3&gt; getestet</t>
-  </si>
-  <si>
     <t>Overkill</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Overkill feature 1&gt; erledigt und gemerged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Overkill feature 1&gt; getestet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    &lt;Overkill feature 2&gt; erledigt und gemerged</t>
   </si>
   <si>
     <t xml:space="preserve">    &lt;Overkill feature 2&gt; getestet</t>
@@ -881,12 +818,504 @@
   <si>
     <t>Die Suchfunktion könnte später bisschen verfeinert werden</t>
   </si>
+  <si>
+    <t>Die TCP Verbindung mit mehreren Clients war nicht möglich, aufgrund unübersichtlichkeit wurde das gesamte Projekt neu aufgesetzt.</t>
+  </si>
+  <si>
+    <t>Das Projekt wurde von neu aufgesetzt somit wurde alles verändert</t>
+  </si>
+  <si>
+    <t>Die GUI ist von nun an nicht mehr in seperaten fxml files sondern die GUI wurde Inline codiert</t>
+  </si>
+  <si>
+    <t>Projekt logisch aufgeteilt</t>
+  </si>
+  <si>
+    <t>Für bessere Übersicht wurde das Projekt in mehreren Klassen aufgeteilt ebenso in mehreren Packages</t>
+  </si>
+  <si>
+    <t>GUI Design</t>
+  </si>
+  <si>
+    <t>Für eine aufgeräumte GUI wurde mittels CSS daran gearbeitet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Die GUI musste Inline codiert werden um bessere Kontrolle über die Clients zu haben. </t>
+  </si>
+  <si>
+    <t>GUI neu erstellt als Inline-Code , Chat Anzeige &amp; LogIn Anzeige</t>
+  </si>
+  <si>
+    <t>Must Have Feature: Konversation zwischen Usern</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Konversation zwischen Usern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>Konversation zwischen Usern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>LogIn/Registrierung</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>LogIn/Registrierung</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>Suchfunktion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>Suchfunktion</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>Status Anzeige</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>Status Anzeige</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Userpasswort änder möglichkeit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>Userpasswort änder möglichkeit</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>Profilbild</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Konversation laden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Profilbild </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Konversation laden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Nachrichtensuchfunktion im Chatt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Nachrichtensuchfunktion im Chatt</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Zeitanzeige beim Nachricht </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Zeitanzeige beim Nachricht</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve">Emojis </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">    </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t>Emojis</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> getestet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">   </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> Bilder senden</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&quot;Arial&quot;"/>
+      </rPr>
+      <t xml:space="preserve"> erledigt und gemerged</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -1010,6 +1439,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="&quot;Arial&quot;"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1041,7 +1476,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -1121,6 +1556,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1390,8 +1829,8 @@
   </sheetPr>
   <dimension ref="B1:C1050"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1449,25 +1888,33 @@
       </c>
     </row>
     <row r="8" spans="2:3" ht="12.75">
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C8" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="12.75">
-      <c r="B9" s="3"/>
+      <c r="B9" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C9" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:3" ht="12.75">
-      <c r="B10" s="3"/>
+      <c r="B10" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C10" s="2" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="12.75">
-      <c r="B11" s="3"/>
+      <c r="B11" s="33" t="s">
+        <v>6</v>
+      </c>
       <c r="C11" s="2" t="s">
         <v>15</v>
       </c>
@@ -1491,19 +1938,25 @@
       </c>
     </row>
     <row r="15" spans="2:3" ht="12.75">
-      <c r="B15" s="3"/>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C15" s="7" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="12.75">
-      <c r="B16" s="3"/>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C16" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="12.75">
-      <c r="B17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C17" s="7" t="s">
         <v>21</v>
       </c>
@@ -1515,213 +1968,229 @@
       </c>
     </row>
     <row r="19" spans="2:3" ht="12.75">
-      <c r="B19" s="3"/>
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C19" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="12.75">
-      <c r="B20" s="3"/>
+      <c r="B20" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C20" s="7" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="12.75">
-      <c r="B21" s="3"/>
+      <c r="B21" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C21" s="7" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="22" spans="2:3" ht="12.75">
-      <c r="B22" s="3"/>
+      <c r="B22" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C22" s="7" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="12.75">
-      <c r="B23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C23" s="7" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="12.75">
-      <c r="B24" s="3"/>
+      <c r="B24" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C24" s="7" t="s">
-        <v>28</v>
+        <v>149</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="12.75">
-      <c r="B25" s="3"/>
+      <c r="B25" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C25" s="7" t="s">
-        <v>29</v>
+        <v>148</v>
       </c>
     </row>
     <row r="26" spans="2:3" ht="12.75">
-      <c r="B26" s="3"/>
+      <c r="B26" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C26" s="7" t="s">
-        <v>30</v>
+        <v>150</v>
       </c>
     </row>
     <row r="27" spans="2:3" ht="12.75">
       <c r="B27" s="3"/>
       <c r="C27" s="7" t="s">
-        <v>31</v>
+        <v>151</v>
       </c>
     </row>
     <row r="28" spans="2:3" ht="12.75">
       <c r="B28" s="3"/>
       <c r="C28" s="7" t="s">
-        <v>32</v>
+        <v>152</v>
       </c>
     </row>
     <row r="29" spans="2:3" ht="12.75">
       <c r="B29" s="3"/>
       <c r="C29" s="7" t="s">
-        <v>33</v>
+        <v>153</v>
       </c>
     </row>
     <row r="30" spans="2:3" ht="12.75">
       <c r="B30" s="5"/>
       <c r="C30" s="8" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="31" spans="2:3" ht="12.75">
       <c r="B31" s="3"/>
       <c r="C31" s="7" t="s">
-        <v>35</v>
+        <v>154</v>
       </c>
     </row>
     <row r="32" spans="2:3" ht="12.75">
       <c r="B32" s="3"/>
       <c r="C32" s="7" t="s">
-        <v>36</v>
+        <v>155</v>
       </c>
     </row>
     <row r="33" spans="2:3" ht="12.75">
       <c r="B33" s="3"/>
       <c r="C33" s="7" t="s">
-        <v>37</v>
+        <v>156</v>
       </c>
     </row>
     <row r="34" spans="2:3" ht="12.75">
       <c r="B34" s="3"/>
       <c r="C34" s="7" t="s">
-        <v>38</v>
+        <v>157</v>
       </c>
     </row>
     <row r="35" spans="2:3" ht="12.75">
       <c r="B35" s="3"/>
       <c r="C35" s="7" t="s">
-        <v>39</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="2:3" ht="12.75">
       <c r="B36" s="3"/>
       <c r="C36" s="7" t="s">
-        <v>40</v>
+        <v>165</v>
       </c>
     </row>
     <row r="37" spans="2:3" ht="12.75">
       <c r="B37" s="5"/>
       <c r="C37" s="8" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="38" spans="2:3" ht="12.75">
       <c r="B38" s="3"/>
       <c r="C38" s="7" t="s">
-        <v>42</v>
+        <v>158</v>
       </c>
     </row>
     <row r="39" spans="2:3" ht="12.75">
       <c r="B39" s="3"/>
       <c r="C39" s="7" t="s">
-        <v>43</v>
+        <v>160</v>
       </c>
     </row>
     <row r="40" spans="2:3" ht="12.75">
       <c r="B40" s="3"/>
       <c r="C40" s="7" t="s">
-        <v>44</v>
+        <v>159</v>
       </c>
     </row>
     <row r="41" spans="2:3" ht="12.75">
       <c r="B41" s="3"/>
       <c r="C41" s="7" t="s">
-        <v>45</v>
+        <v>161</v>
       </c>
     </row>
     <row r="42" spans="2:3" ht="12.75">
       <c r="B42" s="3"/>
       <c r="C42" s="7" t="s">
-        <v>46</v>
+        <v>162</v>
       </c>
     </row>
     <row r="43" spans="2:3" ht="12.75">
       <c r="B43" s="3"/>
       <c r="C43" s="7" t="s">
-        <v>47</v>
+        <v>163</v>
       </c>
     </row>
     <row r="44" spans="2:3" ht="12.75">
       <c r="B44" s="5"/>
       <c r="C44" s="8" t="s">
-        <v>48</v>
+        <v>30</v>
       </c>
     </row>
     <row r="45" spans="2:3" ht="12.75">
       <c r="B45" s="3"/>
       <c r="C45" s="7" t="s">
-        <v>49</v>
+        <v>166</v>
       </c>
     </row>
     <row r="46" spans="2:3" ht="12.75">
       <c r="B46" s="3"/>
       <c r="C46" s="7" t="s">
-        <v>50</v>
+        <v>167</v>
       </c>
     </row>
     <row r="47" spans="2:3" ht="12.75">
       <c r="B47" s="3"/>
       <c r="C47" s="7" t="s">
-        <v>51</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="2:3" ht="12.75">
       <c r="B48" s="3"/>
       <c r="C48" s="7" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
     </row>
     <row r="49" spans="2:3" ht="12.75">
       <c r="B49" s="3"/>
       <c r="C49" s="7" t="s">
-        <v>53</v>
+        <v>32</v>
       </c>
     </row>
     <row r="50" spans="2:3" ht="12.75">
       <c r="B50" s="3"/>
       <c r="C50" s="7" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="12.75">
       <c r="B51" s="5"/>
       <c r="C51" s="8" t="s">
-        <v>55</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="2:3" ht="12.75">
       <c r="B52" s="3"/>
       <c r="C52" s="7" t="s">
-        <v>56</v>
+        <v>35</v>
       </c>
     </row>
     <row r="53" spans="2:3" ht="12.75">
       <c r="B53" s="3"/>
       <c r="C53" s="7" t="s">
-        <v>57</v>
+        <v>36</v>
       </c>
     </row>
     <row r="54" spans="2:3" ht="12.75">
@@ -4717,6 +5186,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4728,7 +5198,7 @@
   <dimension ref="B1:C1001"/>
   <sheetViews>
     <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -4744,54 +5214,54 @@
     </row>
     <row r="2" spans="2:3" ht="12.75">
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C2" s="15" t="s">
-        <v>134</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="61.5" customHeight="1">
       <c r="B3" s="9" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>130</v>
+        <v>109</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="12.75">
       <c r="B4" s="29" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>133</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="12.75">
       <c r="B5" s="30"/>
       <c r="C5" s="15" t="s">
-        <v>132</v>
+        <v>111</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="12.75">
       <c r="B6" s="30"/>
       <c r="C6" s="15" t="s">
-        <v>131</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="25.5">
       <c r="B7" s="9" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>129</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="25.5">
       <c r="B8" s="9" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="12.75">
@@ -4800,22 +5270,22 @@
     </row>
     <row r="10" spans="2:3" ht="12.75">
       <c r="B10" s="29" t="s">
-        <v>64</v>
+        <v>43</v>
       </c>
       <c r="C10" s="18" t="s">
-        <v>119</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="28.5">
       <c r="B11" s="30"/>
       <c r="C11" s="19" t="s">
-        <v>120</v>
+        <v>99</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="14.25">
       <c r="B12" s="30"/>
       <c r="C12" s="19" t="s">
-        <v>121</v>
+        <v>100</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="12.75">
@@ -4824,22 +5294,22 @@
     </row>
     <row r="14" spans="2:3" ht="14.25">
       <c r="B14" s="29" t="s">
-        <v>65</v>
+        <v>44</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="14.25">
       <c r="B15" s="30"/>
       <c r="C15" s="19" t="s">
-        <v>122</v>
+        <v>101</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="14.25">
       <c r="B16" s="30"/>
       <c r="C16" s="19" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="12.75">
@@ -4848,22 +5318,22 @@
     </row>
     <row r="18" spans="2:3" ht="14.25">
       <c r="B18" s="29" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="14.25">
       <c r="B19" s="30"/>
       <c r="C19" s="19" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="14.25">
       <c r="B20" s="30"/>
       <c r="C20" s="19" t="s">
-        <v>125</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="12.75">
@@ -4872,22 +5342,22 @@
     </row>
     <row r="22" spans="2:3" ht="14.25">
       <c r="B22" s="29" t="s">
-        <v>67</v>
+        <v>46</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>126</v>
+        <v>105</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="28.5">
       <c r="B23" s="30"/>
       <c r="C23" s="19" t="s">
-        <v>127</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="14.25">
       <c r="B24" s="30"/>
       <c r="C24" s="19" t="s">
-        <v>128</v>
+        <v>107</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="12.75">
@@ -8822,7 +9292,7 @@
   <dimension ref="B1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8838,84 +9308,87 @@
     <row r="1" spans="2:7" s="21" customFormat="1" ht="12.6" customHeight="1"/>
     <row r="2" spans="2:7" s="24" customFormat="1" ht="12.75">
       <c r="B2" s="23" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C2" s="23" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D2" s="23" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E2" s="23" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="F2" s="23" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="G2" s="23" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:7" s="24" customFormat="1" ht="25.5">
       <c r="B3" s="24" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="D3" s="22" t="s">
-        <v>146</v>
+        <v>125</v>
+      </c>
+      <c r="E3" s="24">
+        <v>2</v>
       </c>
       <c r="F3" s="22" t="s">
-        <v>147</v>
+        <v>117</v>
       </c>
     </row>
     <row r="4" spans="2:7" s="24" customFormat="1" ht="38.25">
       <c r="B4" s="22" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="C4" s="25" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>148</v>
+        <v>127</v>
       </c>
       <c r="E4" s="24">
         <v>5</v>
       </c>
       <c r="F4" s="22" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="G4" s="22" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="2:7" s="24" customFormat="1" ht="25.5">
       <c r="B5" s="24" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="D5" s="22" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="F5" s="22" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="2:7" s="24" customFormat="1" ht="25.5">
       <c r="B6" s="22" t="s">
-        <v>136</v>
+        <v>115</v>
       </c>
       <c r="C6" s="26" t="s">
-        <v>141</v>
+        <v>120</v>
       </c>
       <c r="D6" s="22" t="s">
-        <v>144</v>
+        <v>123</v>
       </c>
       <c r="F6" s="22" t="s">
-        <v>147</v>
+        <v>126</v>
       </c>
     </row>
   </sheetData>
@@ -8928,10 +9401,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="B1:G13"/>
+  <dimension ref="B1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="G7" activeCellId="1" sqref="H4 G7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -8939,119 +9412,135 @@
     <col min="1" max="1" width="3" customWidth="1"/>
     <col min="3" max="3" width="34.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="76.42578125" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27" style="28" customWidth="1"/>
     <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="50.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="2" spans="2:7" s="28" customFormat="1" ht="12.75">
+    <row r="1" spans="2:8" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="2" spans="2:8" s="28" customFormat="1" ht="12.75">
       <c r="B2" s="27" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="27" t="s">
-        <v>69</v>
+        <v>47</v>
+      </c>
+      <c r="C2" s="23" t="s">
+        <v>47</v>
       </c>
       <c r="D2" s="27" t="s">
-        <v>70</v>
+        <v>48</v>
       </c>
       <c r="E2" s="27" t="s">
-        <v>71</v>
+        <v>49</v>
       </c>
       <c r="F2" s="27" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="G2" s="27" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="3" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1">
+        <v>51</v>
+      </c>
+      <c r="H2" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" s="28" customFormat="1" ht="25.5">
       <c r="B3" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>128</v>
+      </c>
+      <c r="E3" s="28" t="s">
+        <v>130</v>
+      </c>
+      <c r="F3" s="28">
+        <v>2</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" s="28" customFormat="1" ht="25.5">
+      <c r="B4" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>129</v>
+      </c>
+      <c r="E4" s="28" t="s">
+        <v>136</v>
+      </c>
+      <c r="F4" s="28">
+        <v>1</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="H4" s="28" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" s="28" customFormat="1" ht="51">
+      <c r="B5" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>133</v>
+      </c>
+      <c r="E5" s="28" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" s="28">
+        <v>1</v>
+      </c>
+      <c r="G5" s="28" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="28" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="28" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" s="28" t="s">
-        <v>151</v>
-      </c>
-      <c r="E3" s="28">
+    </row>
+    <row r="6" spans="2:8" s="28" customFormat="1" ht="38.25">
+      <c r="B6" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>114</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>119</v>
+      </c>
+      <c r="E6" s="22" t="s">
+        <v>125</v>
+      </c>
+      <c r="F6" s="28">
         <v>2</v>
       </c>
-      <c r="F3" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="G3" s="28" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="4" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B4" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>150</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>157</v>
-      </c>
-      <c r="E4" s="28">
-        <v>1</v>
-      </c>
-      <c r="F4" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="G4" s="28" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="5" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B5" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>154</v>
-      </c>
-      <c r="D5" s="28" t="s">
-        <v>155</v>
-      </c>
-      <c r="E5" s="28">
-        <v>1</v>
-      </c>
-      <c r="F5" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="G5" s="28" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="6" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1">
-      <c r="B6" s="28" t="s">
-        <v>135</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>140</v>
-      </c>
-      <c r="D6" s="22" t="s">
-        <v>146</v>
-      </c>
-      <c r="E6" s="28">
-        <v>2</v>
-      </c>
-      <c r="F6" s="28" t="s">
-        <v>138</v>
-      </c>
       <c r="G6" s="28" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="7" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="8" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="9" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="10" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="11" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="12" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
-    <row r="13" spans="2:7" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+        <v>117</v>
+      </c>
+      <c r="H6" s="28" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="8" spans="2:8" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="9" spans="2:8" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="10" spans="2:8" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="11" spans="2:8" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="12" spans="2:8" s="28" customFormat="1" ht="15.75" customHeight="1"/>
+    <row r="13" spans="2:8" s="28" customFormat="1" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -9062,9 +9551,134 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="B2:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="3" customWidth="1"/>
+    <col min="3" max="3" width="77.5703125" style="28" customWidth="1"/>
+    <col min="4" max="4" width="93.7109375" style="28" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="40.28515625" style="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="12.75">
+      <c r="B2" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C2" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="E2" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F2" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="G2" s="27" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="2:7" ht="25.5">
+      <c r="B3" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="28" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>138</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="28" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="4" spans="2:7" ht="38.25">
+      <c r="B4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" s="28" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4">
+        <v>5</v>
+      </c>
+      <c r="F4" t="s">
+        <v>117</v>
+      </c>
+      <c r="G4" s="28" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="5" spans="2:7" ht="12.75">
+      <c r="B5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C5" s="28" t="s">
+        <v>141</v>
+      </c>
+      <c r="D5" s="28" t="s">
+        <v>142</v>
+      </c>
+      <c r="E5">
+        <v>3</v>
+      </c>
+      <c r="F5" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C6" s="28" t="s">
+        <v>143</v>
+      </c>
+      <c r="D6" s="28" t="s">
+        <v>144</v>
+      </c>
+      <c r="E6">
+        <v>4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="7" spans="2:7" ht="15.75" customHeight="1">
+      <c r="B7" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
   <dimension ref="B2:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
@@ -9077,65 +9691,22 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="12" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>73</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="B2:G2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="6.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="29.7109375" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:7">
-      <c r="B2" s="12" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="12" t="s">
-        <v>69</v>
-      </c>
-      <c r="D2" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E2" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="G2" s="12" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
   </sheetData>
@@ -9167,54 +9738,54 @@
     </row>
     <row r="2" spans="2:3" ht="12.75">
       <c r="B2" s="9" t="s">
-        <v>58</v>
+        <v>37</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="3" spans="2:3" ht="61.5" customHeight="1">
       <c r="B3" s="9" t="s">
-        <v>59</v>
+        <v>38</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>75</v>
+        <v>54</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="12.75">
       <c r="B4" s="29" t="s">
-        <v>60</v>
+        <v>39</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>76</v>
+        <v>55</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="12.75">
       <c r="B5" s="30"/>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>56</v>
       </c>
     </row>
     <row r="6" spans="2:3" ht="12.75">
       <c r="B6" s="30"/>
       <c r="C6" s="2" t="s">
-        <v>78</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="2:3" ht="12.75">
       <c r="B7" s="9" t="s">
-        <v>61</v>
+        <v>40</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>79</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="2:3" ht="12.75">
       <c r="B8" s="9" t="s">
-        <v>62</v>
+        <v>41</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>80</v>
+        <v>59</v>
       </c>
     </row>
     <row r="9" spans="2:3" ht="12.75">
@@ -9223,22 +9794,22 @@
     </row>
     <row r="10" spans="2:3" ht="12.75">
       <c r="B10" s="31" t="s">
-        <v>115</v>
+        <v>94</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
     </row>
     <row r="11" spans="2:3" ht="12.75">
       <c r="B11" s="30"/>
       <c r="C11" s="10" t="s">
-        <v>82</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" spans="2:3" ht="12.75">
       <c r="B12" s="30"/>
       <c r="C12" s="10" t="s">
-        <v>83</v>
+        <v>62</v>
       </c>
     </row>
     <row r="13" spans="2:3" ht="12.75">
@@ -9247,22 +9818,22 @@
     </row>
     <row r="14" spans="2:3" ht="12.75">
       <c r="B14" s="31" t="s">
-        <v>116</v>
+        <v>95</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>84</v>
+        <v>63</v>
       </c>
     </row>
     <row r="15" spans="2:3" ht="12.75">
       <c r="B15" s="30"/>
       <c r="C15" s="2" t="s">
-        <v>85</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="2:3" ht="12.75">
       <c r="B16" s="30"/>
       <c r="C16" s="2" t="s">
-        <v>86</v>
+        <v>65</v>
       </c>
     </row>
     <row r="17" spans="2:3" ht="15.75" customHeight="1">
@@ -9270,22 +9841,22 @@
     </row>
     <row r="18" spans="2:3" ht="12.75">
       <c r="B18" s="31" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>87</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="2:3" ht="12.75">
       <c r="B19" s="30"/>
       <c r="C19" s="2" t="s">
-        <v>88</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="2:3" ht="12.75">
       <c r="B20" s="30"/>
       <c r="C20" s="2" t="s">
-        <v>89</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="2:3" ht="15.75" customHeight="1">
@@ -9293,22 +9864,22 @@
     </row>
     <row r="22" spans="2:3" ht="12.75">
       <c r="B22" s="31" t="s">
-        <v>118</v>
+        <v>97</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>90</v>
+        <v>69</v>
       </c>
     </row>
     <row r="23" spans="2:3" ht="12.75">
       <c r="B23" s="30"/>
       <c r="C23" s="2" t="s">
-        <v>91</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" spans="2:3" ht="12.75">
       <c r="B24" s="30"/>
       <c r="C24" s="2" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
     </row>
     <row r="25" spans="2:3" ht="15.75" customHeight="1">
@@ -13255,183 +13826,183 @@
   <sheetData>
     <row r="2" spans="2:7">
       <c r="B2" s="12" t="s">
-        <v>68</v>
+        <v>47</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>69</v>
+        <v>48</v>
       </c>
       <c r="D2" s="12" t="s">
-        <v>70</v>
+        <v>49</v>
       </c>
       <c r="E2" s="12" t="s">
-        <v>71</v>
+        <v>50</v>
       </c>
       <c r="F2" s="12" t="s">
-        <v>72</v>
+        <v>51</v>
       </c>
       <c r="G2" s="12" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="2:7">
       <c r="B3" s="2" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="E3" s="2">
         <v>1.5</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="2:7">
       <c r="B4" s="2" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>96</v>
+        <v>75</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="E4" s="2">
         <v>0.5</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:7">
       <c r="B5" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>99</v>
+        <v>78</v>
       </c>
       <c r="E5" s="2">
         <v>0.25</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="2:7">
       <c r="B6" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>101</v>
+        <v>80</v>
       </c>
       <c r="E6" s="2">
         <v>1.5</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="2:7">
       <c r="B7" s="2" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>103</v>
+        <v>82</v>
       </c>
       <c r="E7" s="2">
         <v>0.5</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>104</v>
+        <v>83</v>
       </c>
       <c r="G7" s="2" t="s">
-        <v>105</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="2:7">
       <c r="B8" s="2" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="E8" s="2">
         <v>2</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="2:7">
       <c r="B9" s="2" t="s">
-        <v>102</v>
+        <v>81</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>108</v>
+        <v>87</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
       </c>
       <c r="E9" s="2">
         <v>1</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="G9" s="2" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="2:7">
       <c r="B10" s="2" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E10" s="2">
         <v>2</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="2:7">
       <c r="B11" s="2" t="s">
-        <v>98</v>
+        <v>77</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E11" s="2">
         <v>2</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="2:7">
       <c r="B12" s="2" t="s">
-        <v>112</v>
+        <v>91</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>111</v>
+        <v>90</v>
       </c>
       <c r="E12" s="2">
         <v>2</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>113</v>
+        <v>92</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>114</v>
+        <v>93</v>
       </c>
     </row>
   </sheetData>

</xml_diff>